<commit_message>
* add report creation
</commit_message>
<xml_diff>
--- a/resources/input/home.xlsx
+++ b/resources/input/home.xlsx
@@ -8,21 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EADA47-16BF-4A2B-A658-604CA2E48C96}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE26E7E7-228F-433C-AD09-B1F17075D021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7170" yWindow="2280" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="test" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
   <si>
     <t>remarks</t>
   </si>
@@ -44,9 +43,6 @@
     <t>test_id</t>
   </si>
   <si>
-    <t>Test_020</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -207,13 +203,28 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>tc_001</t>
+  </si>
+  <si>
+    <t>tc_002</t>
+  </si>
+  <si>
+    <t>tc_003</t>
+  </si>
+  <si>
+    <t>tc_004</t>
+  </si>
+  <si>
+    <t>tc_005</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,6 +242,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -597,40 +614,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BC6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="47.06640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.73046875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.19921875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.9296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.9296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="18.1328125" customWidth="1"/>
-    <col min="20" max="20" width="14.3984375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.86328125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.46484375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.9296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
+    <col min="16" max="19" width="18.140625" customWidth="1"/>
+    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.53125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
@@ -642,70 +659,70 @@
         <v>3</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>52</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="Y1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="Z1" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="AA1" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
@@ -735,205 +752,386 @@
       <c r="BB1" s="3"/>
       <c r="BC1" s="3"/>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
       <c r="F2" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
-        <v>6</v>
-      </c>
       <c r="K2" t="s">
+        <v>4</v>
+      </c>
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
       <c r="F3" t="s">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="M3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
       <c r="T3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="O4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="P4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="U4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="V4" t="s">
+        <v>33</v>
+      </c>
+      <c r="W4" t="s">
         <v>34</v>
       </c>
-      <c r="W4" t="s">
-        <v>35</v>
-      </c>
       <c r="X4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="Y4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="Z4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA4" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB4" t="s">
         <v>44</v>
       </c>
-      <c r="AB4" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R5" t="s">
+        <v>4</v>
+      </c>
+      <c r="S5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>4</v>
+      </c>
+      <c r="R6" t="s">
+        <v>4</v>
+      </c>
+      <c r="S6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{A8A1E9E0-0366-4B9A-A16A-8DB90F1986AD}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{703A5CA8-A6FE-4FA3-A658-CF97999E55B0}"/>
+    <hyperlink ref="N3" r:id="rId3" xr:uid="{31CC35B4-114A-43AB-8661-2A7567BF94F9}"/>
+    <hyperlink ref="P3" r:id="rId4" xr:uid="{83ED797E-211C-4EC3-9513-5129D3C35ED8}"/>
+    <hyperlink ref="D4" r:id="rId5" xr:uid="{68427389-69CF-4E0A-878F-EA2B71930F3C}"/>
+    <hyperlink ref="N4" r:id="rId6" xr:uid="{02D83F37-E55E-4ED1-954B-563D133C141C}"/>
+    <hyperlink ref="P4" r:id="rId7" xr:uid="{C7A8B28E-5323-47D2-A545-82653F3DB894}"/>
+    <hyperlink ref="D5" r:id="rId8" xr:uid="{B798E29D-144F-4114-A189-81DC6038D3A4}"/>
+    <hyperlink ref="D6" r:id="rId9" xr:uid="{A9D8F47C-5B62-4523-A5F6-0438FDD3DA3F}"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758CD1E7-461B-4A22-9ED3-5888DDD38ECB}">
+  <dimension ref="A1:AB4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A1" s="1">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" t="s">
+        <v>23</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="T2" t="s">
+        <v>27</v>
+      </c>
+      <c r="U2" t="s">
+        <v>31</v>
+      </c>
+      <c r="V2" t="s">
+        <v>33</v>
+      </c>
+      <c r="W2" t="s">
+        <v>34</v>
+      </c>
+      <c r="X2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>40</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3" t="s">
         <v>48</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F3" t="s">
         <v>49</v>
       </c>
-      <c r="F5" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="Q3" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" t="s">
+        <v>4</v>
+      </c>
+      <c r="S3" t="s">
         <v>5</v>
       </c>
-      <c r="R5" t="s">
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" t="s">
         <v>5</v>
       </c>
-      <c r="S5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="Q4" t="s">
+        <v>4</v>
+      </c>
+      <c r="R4" t="s">
+        <v>4</v>
+      </c>
+      <c r="S4" t="s">
         <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>5</v>
-      </c>
-      <c r="R6" t="s">
-        <v>5</v>
-      </c>
-      <c r="S6" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{A8A1E9E0-0366-4B9A-A16A-8DB90F1986AD}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{DE26B5E2-7355-41FC-B495-A58F449C49A0}"/>
-    <hyperlink ref="N3" r:id="rId3" xr:uid="{1AF4D662-8106-42E0-B4EB-4F49BDBFCED7}"/>
-    <hyperlink ref="P3" r:id="rId4" xr:uid="{C477A154-8CCE-4792-AB3A-23ABAB2F88D1}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{6F7269BC-8A45-4676-B379-8345D6F5714A}"/>
-    <hyperlink ref="N4" r:id="rId6" xr:uid="{9998DE4F-3899-463C-95EA-5D8DFA8E3038}"/>
-    <hyperlink ref="P4" r:id="rId7" xr:uid="{1FB7ADAC-E2BF-42CD-B0A0-C47E4D101D3F}"/>
-    <hyperlink ref="D5" r:id="rId8" xr:uid="{EF78C92F-D7BF-43A9-9212-C31247E83D13}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{E72A2B86-B15E-4A90-92CB-22B069AE70C5}"/>
+    <hyperlink ref="D1" r:id="rId1" xr:uid="{DE26B5E2-7355-41FC-B495-A58F449C49A0}"/>
+    <hyperlink ref="N1" r:id="rId2" xr:uid="{1AF4D662-8106-42E0-B4EB-4F49BDBFCED7}"/>
+    <hyperlink ref="P1" r:id="rId3" xr:uid="{C477A154-8CCE-4792-AB3A-23ABAB2F88D1}"/>
+    <hyperlink ref="D2" r:id="rId4" xr:uid="{6F7269BC-8A45-4676-B379-8345D6F5714A}"/>
+    <hyperlink ref="N2" r:id="rId5" xr:uid="{9998DE4F-3899-463C-95EA-5D8DFA8E3038}"/>
+    <hyperlink ref="P2" r:id="rId6" xr:uid="{1FB7ADAC-E2BF-42CD-B0A0-C47E4D101D3F}"/>
+    <hyperlink ref="D3" r:id="rId7" xr:uid="{EF78C92F-D7BF-43A9-9212-C31247E83D13}"/>
+    <hyperlink ref="D4" r:id="rId8" xr:uid="{E72A2B86-B15E-4A90-92CB-22B069AE70C5}"/>
   </hyperlinks>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
* support additional columns, spread files
</commit_message>
<xml_diff>
--- a/resources/input/home.xlsx
+++ b/resources/input/home.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\TestFactory\resources\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobyt\Projects\TestFactory\resources\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE26E7E7-228F-433C-AD09-B1F17075D021}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80B8CB50-0200-4411-8E64-5251D991C2C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7170" yWindow="2280" windowWidth="21600" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="64">
   <si>
     <t>remarks</t>
   </si>
@@ -218,6 +218,9 @@
   </si>
   <si>
     <t>tc_005</t>
+  </si>
+  <si>
+    <t>ticket</t>
   </si>
 </sst>
 </file>
@@ -612,34 +615,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BC6"/>
+  <dimension ref="A1:BD6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="19" width="18.140625" customWidth="1"/>
-    <col min="20" max="20" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="13" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47" customWidth="1"/>
+    <col min="4" max="4" width="24" customWidth="1"/>
+    <col min="5" max="5" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="20" width="18.140625" customWidth="1"/>
+    <col min="21" max="21" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="16" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>57</v>
       </c>
@@ -647,84 +651,86 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
       <c r="AF1" s="1"/>
@@ -749,208 +755,224 @@
       <c r="AY1" s="1"/>
       <c r="AZ1" s="1"/>
       <c r="BA1" s="1"/>
-      <c r="BB1" s="3"/>
+      <c r="BB1" s="1"/>
       <c r="BC1" s="3"/>
+      <c r="BD1" s="3"/>
     </row>
-    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>123123</v>
+      </c>
+      <c r="D2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>58</v>
       </c>
-      <c r="I2" t="s">
-        <v>4</v>
-      </c>
       <c r="J2" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="K2" t="s">
-        <v>4</v>
-      </c>
       <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C3">
+        <v>4123123</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>59</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>19</v>
       </c>
-      <c r="N3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>23</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="Q3" s="2"/>
       <c r="R3" s="2"/>
       <c r="S3" s="2"/>
-      <c r="T3" t="s">
+      <c r="T3" s="2"/>
+      <c r="U3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>124512</v>
+      </c>
+      <c r="D4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>60</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>19</v>
       </c>
-      <c r="N4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>23</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>27</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>31</v>
       </c>
-      <c r="V4" t="s">
+      <c r="W4" t="s">
         <v>33</v>
       </c>
-      <c r="W4" t="s">
+      <c r="X4" t="s">
         <v>34</v>
       </c>
-      <c r="X4" t="s">
+      <c r="Y4" t="s">
         <v>36</v>
       </c>
-      <c r="Y4" t="s">
+      <c r="Z4" t="s">
         <v>38</v>
       </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>40</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>43</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="5" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5">
+        <v>32313</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>48</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>61</v>
       </c>
-      <c r="Q5" t="s">
-        <v>4</v>
-      </c>
       <c r="R5" t="s">
         <v>4</v>
       </c>
       <c r="S5" t="s">
+        <v>4</v>
+      </c>
+      <c r="T5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:55" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="C6">
+        <v>2341243</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>54</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>62</v>
       </c>
-      <c r="G6" t="s">
-        <v>4</v>
-      </c>
       <c r="H6" t="s">
+        <v>4</v>
+      </c>
+      <c r="I6" t="s">
         <v>5</v>
       </c>
-      <c r="Q6" t="s">
-        <v>4</v>
-      </c>
       <c r="R6" t="s">
         <v>4</v>
       </c>
       <c r="S6" t="s">
+        <v>4</v>
+      </c>
+      <c r="T6" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{A8A1E9E0-0366-4B9A-A16A-8DB90F1986AD}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{703A5CA8-A6FE-4FA3-A658-CF97999E55B0}"/>
-    <hyperlink ref="N3" r:id="rId3" xr:uid="{31CC35B4-114A-43AB-8661-2A7567BF94F9}"/>
-    <hyperlink ref="P3" r:id="rId4" xr:uid="{83ED797E-211C-4EC3-9513-5129D3C35ED8}"/>
-    <hyperlink ref="D4" r:id="rId5" xr:uid="{68427389-69CF-4E0A-878F-EA2B71930F3C}"/>
-    <hyperlink ref="N4" r:id="rId6" xr:uid="{02D83F37-E55E-4ED1-954B-563D133C141C}"/>
-    <hyperlink ref="P4" r:id="rId7" xr:uid="{C7A8B28E-5323-47D2-A545-82653F3DB894}"/>
-    <hyperlink ref="D5" r:id="rId8" xr:uid="{B798E29D-144F-4114-A189-81DC6038D3A4}"/>
-    <hyperlink ref="D6" r:id="rId9" xr:uid="{A9D8F47C-5B62-4523-A5F6-0438FDD3DA3F}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A8A1E9E0-0366-4B9A-A16A-8DB90F1986AD}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{703A5CA8-A6FE-4FA3-A658-CF97999E55B0}"/>
+    <hyperlink ref="O3" r:id="rId3" xr:uid="{31CC35B4-114A-43AB-8661-2A7567BF94F9}"/>
+    <hyperlink ref="Q3" r:id="rId4" xr:uid="{83ED797E-211C-4EC3-9513-5129D3C35ED8}"/>
+    <hyperlink ref="E4" r:id="rId5" xr:uid="{68427389-69CF-4E0A-878F-EA2B71930F3C}"/>
+    <hyperlink ref="O4" r:id="rId6" xr:uid="{02D83F37-E55E-4ED1-954B-563D133C141C}"/>
+    <hyperlink ref="Q4" r:id="rId7" xr:uid="{C7A8B28E-5323-47D2-A545-82653F3DB894}"/>
+    <hyperlink ref="E5" r:id="rId8" xr:uid="{B798E29D-144F-4114-A189-81DC6038D3A4}"/>
+    <hyperlink ref="E6" r:id="rId9" xr:uid="{A9D8F47C-5B62-4523-A5F6-0438FDD3DA3F}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>